<commit_message>
One more update for clarity (I meant TOS=1 not SIGCOR)
</commit_message>
<xml_diff>
--- a/model-files/scripts/block/Capclass_Speed_Capacity.xlsx
+++ b/model-files/scripts/block/Capclass_Speed_Capacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6.1_develop\model-files\scripts\block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5541F6-4E20-4FBB-9101-24F1EE382A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EAE5DF-DC1D-42DB-B3EE-0540C29883D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="14655" activeTab="2" xr2:uid="{4E95F9D0-AD5A-46FF-95C2-9E879274FEFF}"/>
+    <workbookView xWindow="3645" yWindow="555" windowWidth="28800" windowHeight="14655" activeTab="2" xr2:uid="{4E95F9D0-AD5A-46FF-95C2-9E879274FEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="existing" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
   <si>
     <t>AreaType</t>
   </si>
@@ -186,6 +186,9 @@
   <si>
     <t>ITS Freeway</t>
   </si>
+  <si>
+    <t>+5</t>
+  </si>
 </sst>
 </file>
 
@@ -194,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +266,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -531,9 +541,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,6 +606,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3448,48 +3459,48 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="N2" s="79" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="N2" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
       <c r="Y2" s="23"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
       <c r="N3" s="24" t="s">
         <v>23</v>
       </c>
@@ -3530,10 +3541,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="3">
         <v>1</v>
       </c>
@@ -4090,33 +4101,33 @@
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
-      <c r="N13" s="79" t="s">
+      <c r="N13" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
-      <c r="S13" s="79"/>
-      <c r="T13" s="79"/>
-      <c r="U13" s="79"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="79"/>
-      <c r="X13" s="79"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="78"/>
+      <c r="X13" s="78"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
       <c r="N14" s="24" t="s">
         <v>23</v>
       </c>
@@ -4157,10 +4168,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="78"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="3">
         <v>1</v>
       </c>
@@ -4583,33 +4594,33 @@
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
-      <c r="N24" s="79" t="s">
+      <c r="N24" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
-      <c r="T24" s="79"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="79"/>
-      <c r="W24" s="79"/>
-      <c r="X24" s="79"/>
+      <c r="O24" s="78"/>
+      <c r="P24" s="78"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="78"/>
+      <c r="U24" s="78"/>
+      <c r="V24" s="78"/>
+      <c r="W24" s="78"/>
+      <c r="X24" s="78"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
       <c r="N25" s="24" t="s">
         <v>34</v>
       </c>
@@ -4650,10 +4661,10 @@
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="78"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="3">
         <v>1</v>
       </c>
@@ -6303,7 +6314,7 @@
   <dimension ref="A1:AK38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6316,7 +6327,7 @@
     <col min="15" max="24" width="8" style="1" customWidth="1"/>
     <col min="25" max="25" width="4.42578125" style="1" customWidth="1"/>
     <col min="26" max="26" width="6.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" style="1" customWidth="1"/>
     <col min="28" max="29" width="8.28515625" style="1" customWidth="1"/>
     <col min="30" max="16384" width="14.42578125" style="1"/>
   </cols>
@@ -6327,54 +6338,54 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="N2" s="79" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="N2" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
       <c r="Y2" s="23"/>
-      <c r="Z2" s="79" t="s">
+      <c r="Z2" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
       <c r="N3" s="24" t="s">
         <v>23</v>
       </c>
@@ -6385,7 +6396,7 @@
       <c r="Z3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="65" t="s">
+      <c r="AD3" s="64" t="s">
         <v>46</v>
       </c>
     </row>
@@ -6428,10 +6439,10 @@
       </c>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="3">
         <v>1</v>
       </c>
@@ -6585,15 +6596,15 @@
       <c r="Z6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" s="56">
+      <c r="AA6" s="65">
         <f>W10</f>
         <v>45</v>
       </c>
-      <c r="AB6" s="57">
+      <c r="AB6" s="56">
         <f>W6</f>
         <v>55</v>
       </c>
-      <c r="AC6" s="58">
+      <c r="AC6" s="57">
         <f>X6</f>
         <v>40</v>
       </c>
@@ -6681,15 +6692,15 @@
       <c r="Z7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AA7" s="69">
+      <c r="AA7" s="68">
         <f>W10</f>
         <v>45</v>
       </c>
-      <c r="AB7" s="59">
+      <c r="AB7" s="58">
         <f>W6</f>
         <v>55</v>
       </c>
-      <c r="AC7" s="60">
+      <c r="AC7" s="59">
         <f>X6</f>
         <v>40</v>
       </c>
@@ -6777,15 +6788,15 @@
       <c r="Z8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AA8" s="61">
+      <c r="AA8" s="60">
         <f>W10</f>
         <v>45</v>
       </c>
-      <c r="AB8" s="59">
+      <c r="AB8" s="58">
         <f>W7</f>
         <v>60</v>
       </c>
-      <c r="AC8" s="60">
+      <c r="AC8" s="59">
         <f>X7</f>
         <v>45</v>
       </c>
@@ -6873,15 +6884,15 @@
       <c r="Z9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AA9" s="61">
+      <c r="AA9" s="60">
         <f>W10</f>
         <v>45</v>
       </c>
-      <c r="AB9" s="59">
+      <c r="AB9" s="58">
         <f>W7</f>
         <v>60</v>
       </c>
-      <c r="AC9" s="60">
+      <c r="AC9" s="59">
         <f>X7</f>
         <v>45</v>
       </c>
@@ -6969,15 +6980,15 @@
       <c r="Z10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" s="61">
+      <c r="AA10" s="60">
         <f>W11</f>
         <v>50</v>
       </c>
-      <c r="AB10" s="59">
+      <c r="AB10" s="58">
         <f>W8</f>
         <v>65</v>
       </c>
-      <c r="AC10" s="71">
+      <c r="AC10" s="70">
         <f>X8</f>
         <v>55</v>
       </c>
@@ -7065,15 +7076,15 @@
       <c r="Z11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="AA11" s="62">
+      <c r="AA11" s="61">
         <f>W11</f>
         <v>50</v>
       </c>
-      <c r="AB11" s="63">
+      <c r="AB11" s="62">
         <f>W8</f>
         <v>65</v>
       </c>
-      <c r="AC11" s="64">
+      <c r="AC11" s="63">
         <f>X8</f>
         <v>55</v>
       </c>
@@ -7091,6 +7102,13 @@
       <c r="P12" s="50">
         <v>75</v>
       </c>
+      <c r="AA12" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="D13" s="3"/>
@@ -7102,25 +7120,25 @@
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
-      <c r="N14" s="79" t="s">
+      <c r="N14" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="79"/>
-      <c r="U14" s="79"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="79"/>
-      <c r="X14" s="79"/>
-      <c r="Z14" s="79" t="s">
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
+      <c r="U14" s="78"/>
+      <c r="V14" s="78"/>
+      <c r="W14" s="78"/>
+      <c r="X14" s="78"/>
+      <c r="Z14" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="AA14" s="79"/>
-      <c r="AB14" s="79"/>
-      <c r="AC14" s="79"/>
+      <c r="AA14" s="78"/>
+      <c r="AB14" s="78"/>
+      <c r="AC14" s="78"/>
       <c r="AD14" s="23"/>
       <c r="AE14" s="23"/>
       <c r="AF14" s="23"/>
@@ -7131,18 +7149,18 @@
       <c r="AK14" s="23"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
       <c r="N15" s="24" t="s">
         <v>23</v>
       </c>
@@ -7189,10 +7207,10 @@
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="78"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="3">
         <v>1</v>
       </c>
@@ -7322,15 +7340,15 @@
       <c r="Z18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA18" s="66">
+      <c r="AA18" s="65">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB18" s="67">
+      <c r="AB18" s="66">
         <f>W18</f>
         <v>2100</v>
       </c>
-      <c r="AC18" s="68">
+      <c r="AC18" s="67">
         <f>X18</f>
         <v>1500</v>
       </c>
@@ -7394,15 +7412,15 @@
       <c r="Z19" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AA19" s="69">
+      <c r="AA19" s="68">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB19" s="70">
+      <c r="AB19" s="69">
         <f>W18</f>
         <v>2100</v>
       </c>
-      <c r="AC19" s="71">
+      <c r="AC19" s="70">
         <f>X18</f>
         <v>1500</v>
       </c>
@@ -7466,15 +7484,15 @@
       <c r="Z20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AA20" s="69">
+      <c r="AA20" s="68">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB20" s="70">
+      <c r="AB20" s="69">
         <f>W19</f>
         <v>2150</v>
       </c>
-      <c r="AC20" s="71">
+      <c r="AC20" s="70">
         <f>X19</f>
         <v>1650</v>
       </c>
@@ -7538,15 +7556,15 @@
       <c r="Z21" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AA21" s="69">
+      <c r="AA21" s="68">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB21" s="70">
+      <c r="AB21" s="69">
         <f>W19</f>
         <v>2150</v>
       </c>
-      <c r="AC21" s="71">
+      <c r="AC21" s="70">
         <f>X19</f>
         <v>1650</v>
       </c>
@@ -7610,15 +7628,15 @@
       <c r="Z22" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="AA22" s="69">
+      <c r="AA22" s="68">
         <f>W23</f>
         <v>2050</v>
       </c>
-      <c r="AB22" s="70">
+      <c r="AB22" s="69">
         <f>W20</f>
         <v>2200</v>
       </c>
-      <c r="AC22" s="71">
+      <c r="AC22" s="70">
         <f>X20</f>
         <v>1700</v>
       </c>
@@ -7682,15 +7700,15 @@
       <c r="Z23" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="AA23" s="72">
+      <c r="AA23" s="71">
         <f>W23</f>
         <v>2050</v>
       </c>
-      <c r="AB23" s="73">
+      <c r="AB23" s="72">
         <f>W20</f>
         <v>2200</v>
       </c>
-      <c r="AC23" s="74">
+      <c r="AC23" s="73">
         <f>X20</f>
         <v>1700</v>
       </c>
@@ -7711,28 +7729,28 @@
       <c r="V24" s="31"/>
       <c r="W24" s="31"/>
       <c r="X24" s="31"/>
-      <c r="AA24" s="54" t="s">
+      <c r="AA24" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="AB24" s="55" t="s">
+      <c r="AB24" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="AC24" s="55" t="s">
+      <c r="AC24" s="80" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="N25" s="3"/>
-      <c r="O25" s="75"/>
+      <c r="O25" s="74"/>
       <c r="P25" s="26"/>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="75"/>
-      <c r="S25" s="75"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="75"/>
-      <c r="V25" s="75"/>
-      <c r="W25" s="75"/>
-      <c r="X25" s="75"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
       <c r="AA25" s="54"/>
       <c r="AB25" s="55"/>
       <c r="AC25" s="55"/>
@@ -7743,33 +7761,33 @@
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-      <c r="N26" s="79" t="s">
+      <c r="N26" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="79"/>
-      <c r="U26" s="79"/>
-      <c r="V26" s="79"/>
-      <c r="W26" s="79"/>
-      <c r="X26" s="79"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="78"/>
+      <c r="V26" s="78"/>
+      <c r="W26" s="78"/>
+      <c r="X26" s="78"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
       <c r="N27" s="24" t="s">
         <v>34</v>
       </c>
@@ -7810,10 +7828,10 @@
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="78"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="3">
         <v>1</v>
       </c>
@@ -8206,7 +8224,7 @@
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="N36" s="76" t="s">
+      <c r="N36" s="75" t="s">
         <v>47</v>
       </c>
       <c r="P36" s="52">
@@ -8222,6 +8240,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N26:X26"/>
+    <mergeCell ref="C27:L27"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="N2:X2"/>
@@ -8229,16 +8252,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="N14:X14"/>
     <mergeCell ref="C15:L15"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N26:X26"/>
-    <mergeCell ref="C27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="AB24:AC24" numberStoredAsText="1"/>
+    <ignoredError sqref="AB24:AC24 AA12:AC12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NOP: This file only serves as documentation.
</commit_message>
<xml_diff>
--- a/model-files/scripts/block/Capclass_Speed_Capacity.xlsx
+++ b/model-files/scripts/block/Capclass_Speed_Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-v1.6.1_develop\model-files\scripts\block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EAE5DF-DC1D-42DB-B3EE-0540C29883D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29497B03-81F9-4FEC-A7B4-E5B72DDC2140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="555" windowWidth="28800" windowHeight="14655" activeTab="2" xr2:uid="{4E95F9D0-AD5A-46FF-95C2-9E879274FEFF}"/>
+    <workbookView xWindow="1605" yWindow="1605" windowWidth="18525" windowHeight="10650" activeTab="2" xr2:uid="{4E95F9D0-AD5A-46FF-95C2-9E879274FEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="existing" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="54">
   <si>
     <t>AreaType</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>+5</t>
+  </si>
+  <si>
+    <t>CAPCLASS to SPEED, SIGCOR=1</t>
+  </si>
+  <si>
+    <t>Easier to read version (applies SIGCOR=1 override)</t>
+  </si>
+  <si>
+    <t>CAPCLASS to CAPACITY, SIGCOR=1</t>
+  </si>
+  <si>
+    <t>+50 to +100</t>
   </si>
 </sst>
 </file>
@@ -408,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -565,9 +577,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,6 +608,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,10 +634,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3459,48 +3483,48 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="N2" s="78" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="N2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
       <c r="Y2" s="23"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
       <c r="N3" s="24" t="s">
         <v>23</v>
       </c>
@@ -3541,10 +3565,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="77"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="3">
         <v>1</v>
       </c>
@@ -4101,33 +4125,33 @@
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
-      <c r="N13" s="78" t="s">
+      <c r="N13" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="78"/>
-      <c r="X13" s="78"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="84"/>
+      <c r="T13" s="84"/>
+      <c r="U13" s="84"/>
+      <c r="V13" s="84"/>
+      <c r="W13" s="84"/>
+      <c r="X13" s="84"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
       <c r="N14" s="24" t="s">
         <v>23</v>
       </c>
@@ -4168,10 +4192,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="77"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="3">
         <v>1</v>
       </c>
@@ -4594,33 +4618,33 @@
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
-      <c r="N24" s="78" t="s">
+      <c r="N24" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="78"/>
-      <c r="V24" s="78"/>
-      <c r="W24" s="78"/>
-      <c r="X24" s="78"/>
+      <c r="O24" s="84"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="84"/>
+      <c r="S24" s="84"/>
+      <c r="T24" s="84"/>
+      <c r="U24" s="84"/>
+      <c r="V24" s="84"/>
+      <c r="W24" s="84"/>
+      <c r="X24" s="84"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
       <c r="N25" s="24" t="s">
         <v>34</v>
       </c>
@@ -4661,10 +4685,10 @@
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="77"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="3">
         <v>1</v>
       </c>
@@ -6313,8 +6337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82F6074-1CB7-466B-B07C-ACE3F13B63C5}">
   <dimension ref="A1:AK38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6329,7 +6353,9 @@
     <col min="26" max="26" width="6.7109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="11.5703125" style="1" customWidth="1"/>
     <col min="28" max="29" width="8.28515625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="14.42578125" style="1"/>
+    <col min="30" max="30" width="7" style="1" customWidth="1"/>
+    <col min="31" max="34" width="10" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
@@ -6338,54 +6364,60 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="N2" s="78" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="N2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
       <c r="Y2" s="23"/>
-      <c r="Z2" s="78" t="s">
+      <c r="Z2" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AE2" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
       <c r="N3" s="24" t="s">
         <v>23</v>
       </c>
@@ -6396,8 +6428,8 @@
       <c r="Z3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="64" t="s">
-        <v>46</v>
+      <c r="AE3" s="24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:37" ht="25.5" x14ac:dyDescent="0.2">
@@ -6437,12 +6469,18 @@
       <c r="AA4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="AF4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="19" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="77"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="3">
         <v>1</v>
       </c>
@@ -6511,6 +6549,12 @@
       </c>
       <c r="AC5" s="3">
         <v>3</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
@@ -6596,7 +6640,7 @@
       <c r="Z6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA6" s="65">
+      <c r="AA6" s="64">
         <f>W10</f>
         <v>45</v>
       </c>
@@ -6608,6 +6652,17 @@
         <f>X6</f>
         <v>40</v>
       </c>
+      <c r="AE6" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF6" s="78">
+        <f>X6</f>
+        <v>40</v>
+      </c>
+      <c r="AG6" s="79">
+        <f>X9</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -6692,7 +6747,7 @@
       <c r="Z7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AA7" s="68">
+      <c r="AA7" s="67">
         <f>W10</f>
         <v>45</v>
       </c>
@@ -6704,6 +6759,17 @@
         <f>X6</f>
         <v>40</v>
       </c>
+      <c r="AE7" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF7" s="60">
+        <f>X6</f>
+        <v>40</v>
+      </c>
+      <c r="AG7" s="29">
+        <f>X9</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -6800,6 +6866,17 @@
         <f>X7</f>
         <v>45</v>
       </c>
+      <c r="AE8" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="60">
+        <f>X7</f>
+        <v>45</v>
+      </c>
+      <c r="AG8" s="29">
+        <f>X10</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -6896,6 +6973,17 @@
         <f>X7</f>
         <v>45</v>
       </c>
+      <c r="AE9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF9" s="60">
+        <f>X7</f>
+        <v>45</v>
+      </c>
+      <c r="AG9" s="29">
+        <f>X10</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -6988,9 +7076,20 @@
         <f>W8</f>
         <v>65</v>
       </c>
-      <c r="AC10" s="70">
+      <c r="AC10" s="69">
         <f>X8</f>
         <v>55</v>
+      </c>
+      <c r="AE10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF10" s="67">
+        <f>X8</f>
+        <v>55</v>
+      </c>
+      <c r="AG10" s="80">
+        <f>X11</f>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
@@ -7088,6 +7187,17 @@
         <f>X8</f>
         <v>55</v>
       </c>
+      <c r="AE11" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF11" s="61">
+        <f>X8</f>
+        <v>55</v>
+      </c>
+      <c r="AG11" s="28">
+        <f>X11</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -7102,11 +7212,17 @@
       <c r="P12" s="50">
         <v>75</v>
       </c>
-      <c r="AA12" s="80" t="s">
+      <c r="AA12" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="AB12" s="80"/>
-      <c r="AC12" s="80" t="s">
+      <c r="AB12" s="76"/>
+      <c r="AC12" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF12" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG12" s="76" t="s">
         <v>49</v>
       </c>
     </row>
@@ -7120,52 +7236,57 @@
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
-      <c r="N14" s="78" t="s">
+      <c r="N14" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="78"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="78"/>
-      <c r="T14" s="78"/>
-      <c r="U14" s="78"/>
-      <c r="V14" s="78"/>
-      <c r="W14" s="78"/>
-      <c r="X14" s="78"/>
-      <c r="Z14" s="78" t="s">
+      <c r="O14" s="84"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="84"/>
+      <c r="S14" s="84"/>
+      <c r="T14" s="84"/>
+      <c r="U14" s="84"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="84"/>
+      <c r="X14" s="84"/>
+      <c r="Z14" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="AA14" s="78"/>
-      <c r="AB14" s="78"/>
-      <c r="AC14" s="78"/>
+      <c r="AA14" s="84"/>
+      <c r="AB14" s="84"/>
+      <c r="AC14" s="84"/>
       <c r="AD14" s="23"/>
-      <c r="AE14" s="23"/>
-      <c r="AF14" s="23"/>
-      <c r="AG14" s="23"/>
-      <c r="AH14" s="23"/>
+      <c r="AE14" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF14" s="84"/>
+      <c r="AG14" s="84"/>
+      <c r="AH14" s="84"/>
       <c r="AI14" s="23"/>
       <c r="AJ14" s="23"/>
       <c r="AK14" s="23"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
       <c r="N15" s="24" t="s">
         <v>23</v>
       </c>
       <c r="Z15" s="24" t="s">
         <v>41</v>
+      </c>
+      <c r="AE15" s="24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="25.5" x14ac:dyDescent="0.2">
@@ -7205,12 +7326,18 @@
       <c r="AA16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A17" s="77" t="s">
+      <c r="AF16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG16" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A17" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="77"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="3">
         <v>1</v>
       </c>
@@ -7280,8 +7407,14 @@
       <c r="AC17" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AF17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -7340,20 +7473,31 @@
       <c r="Z18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AA18" s="65">
+      <c r="AA18" s="64">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB18" s="66">
+      <c r="AB18" s="65">
         <f>W18</f>
         <v>2100</v>
       </c>
-      <c r="AC18" s="67">
+      <c r="AC18" s="66">
         <f>X18</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF18" s="64">
+        <f>X18</f>
+        <v>1500</v>
+      </c>
+      <c r="AG18" s="79">
+        <f>X21</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -7412,20 +7556,31 @@
       <c r="Z19" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AA19" s="68">
+      <c r="AA19" s="67">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB19" s="69">
+      <c r="AB19" s="68">
         <f>W18</f>
         <v>2100</v>
       </c>
-      <c r="AC19" s="70">
+      <c r="AC19" s="69">
         <f>X18</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE19" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF19" s="67">
+        <f>X18</f>
+        <v>1500</v>
+      </c>
+      <c r="AG19" s="80">
+        <f>X21</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -7484,20 +7639,31 @@
       <c r="Z20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AA20" s="68">
+      <c r="AA20" s="67">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB20" s="69">
+      <c r="AB20" s="68">
         <f>W19</f>
         <v>2150</v>
       </c>
-      <c r="AC20" s="70">
+      <c r="AC20" s="69">
         <f>X19</f>
         <v>1650</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE20" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF20" s="67">
+        <f>X19</f>
+        <v>1650</v>
+      </c>
+      <c r="AG20" s="80">
+        <f>X22</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -7556,20 +7722,31 @@
       <c r="Z21" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AA21" s="68">
+      <c r="AA21" s="67">
         <f>W22</f>
         <v>2000</v>
       </c>
-      <c r="AB21" s="69">
+      <c r="AB21" s="68">
         <f>W19</f>
         <v>2150</v>
       </c>
-      <c r="AC21" s="70">
+      <c r="AC21" s="69">
         <f>X19</f>
         <v>1650</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE21" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF21" s="67">
+        <f>X19</f>
+        <v>1650</v>
+      </c>
+      <c r="AG21" s="80">
+        <f>X22</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -7628,20 +7805,31 @@
       <c r="Z22" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="AA22" s="68">
+      <c r="AA22" s="67">
         <f>W23</f>
         <v>2050</v>
       </c>
-      <c r="AB22" s="69">
+      <c r="AB22" s="68">
         <f>W20</f>
         <v>2200</v>
       </c>
-      <c r="AC22" s="70">
+      <c r="AC22" s="69">
         <f>X20</f>
         <v>1700</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE22" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF22" s="67">
+        <f>X20</f>
+        <v>1700</v>
+      </c>
+      <c r="AG22" s="80">
+        <f>X23</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -7700,20 +7888,31 @@
       <c r="Z23" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="AA23" s="71">
+      <c r="AA23" s="70">
         <f>W23</f>
         <v>2050</v>
       </c>
-      <c r="AB23" s="72">
+      <c r="AB23" s="71">
         <f>W20</f>
         <v>2200</v>
       </c>
-      <c r="AC23" s="73">
+      <c r="AC23" s="72">
         <f>X20</f>
         <v>1700</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AE23" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF23" s="70">
+        <f>X20</f>
+        <v>1700</v>
+      </c>
+      <c r="AG23" s="81">
+        <f>X23</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="N24" s="2" t="s">
         <v>47</v>
       </c>
@@ -7729,70 +7928,81 @@
       <c r="V24" s="31"/>
       <c r="W24" s="31"/>
       <c r="X24" s="31"/>
-      <c r="AA24" s="79" t="s">
+      <c r="AA24" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="AB24" s="80" t="s">
+      <c r="AB24" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="AC24" s="80" t="s">
+      <c r="AC24" s="76" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AF24" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG24" s="76" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="N25" s="3"/>
-      <c r="O25" s="74"/>
+      <c r="O25" s="73"/>
       <c r="P25" s="26"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="74"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="73"/>
+      <c r="U25" s="73"/>
+      <c r="V25" s="73"/>
+      <c r="W25" s="73"/>
+      <c r="X25" s="73"/>
       <c r="AA25" s="54"/>
       <c r="AB25" s="55"/>
       <c r="AC25" s="55"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-      <c r="N26" s="78" t="s">
+      <c r="N26" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="78"/>
-      <c r="P26" s="78"/>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="78"/>
-      <c r="S26" s="78"/>
-      <c r="T26" s="78"/>
-      <c r="U26" s="78"/>
-      <c r="V26" s="78"/>
-      <c r="W26" s="78"/>
-      <c r="X26" s="78"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="C27" s="76" t="s">
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
+      <c r="T26" s="84"/>
+      <c r="U26" s="84"/>
+      <c r="V26" s="84"/>
+      <c r="W26" s="84"/>
+      <c r="X26" s="84"/>
+      <c r="Z26" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA26" s="77"/>
+      <c r="AB26" s="77"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C27" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
       <c r="N27" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="19" t="s">
         <v>15</v>
       </c>
@@ -7827,11 +8037,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A29" s="77" t="s">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A29" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="77"/>
+      <c r="B29" s="83"/>
       <c r="C29" s="3">
         <v>1</v>
       </c>
@@ -7893,7 +8103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
@@ -7948,7 +8158,7 @@
         <v>14.125999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -8003,7 +8213,7 @@
         <v>16.48</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -8224,7 +8434,7 @@
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="N36" s="75" t="s">
+      <c r="N36" s="74" t="s">
         <v>47</v>
       </c>
       <c r="P36" s="52">
@@ -8239,12 +8449,9 @@
       <c r="P38" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N26:X26"/>
-    <mergeCell ref="C27:L27"/>
+  <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AE14:AH14"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="N2:X2"/>
@@ -8252,6 +8459,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="N14:X14"/>
     <mergeCell ref="C15:L15"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N26:X26"/>
+    <mergeCell ref="C27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>